<commit_message>
chore:update to contact book
</commit_message>
<xml_diff>
--- a/contact_book/Contact.xlsx
+++ b/contact_book/Contact.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,7 +429,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Number</t>
+          <t>Phone Number</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -441,85 +441,68 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>brian</t>
+          <t>john</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0944782</t>
+          <t>36478291</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>brian@email.com</t>
+          <t>john@email.com</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>jerry</t>
+          <t>brian</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>621894</t>
+          <t>2834501</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>jerry@email.com</t>
+          <t>brian@email.com</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>asingwire</t>
+          <t>judith</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>21123123</t>
+          <t>30981234</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>brian</t>
+          <t>judith@email.com</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>bulma</t>
+          <t>nas</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>12312414</t>
+          <t>378192304</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>bulma</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>david</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>9865428</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>david@example.com</t>
+          <t>nas@email.com</t>
         </is>
       </c>
     </row>

</xml_diff>